<commit_message>
Version 3.5 processor_no_weight: Digital exports will have incorrect Body (HTML) and duplicated SEO logic evaluation.
description.py: The function builds HTML (desc), puts it into context['description'],
and then returns safe_eval(seo_formula, context). This is wrong: the function must return the HTML Body, not the SEO string.
Hardcoded Sterlco block baked into description builder. Violates config‑driven design and makes behavior supplier‑specific.

processor.py: needs upgrade
</commit_message>
<xml_diff>
--- a/Sterlco _4300_Series_Condensate_Duplex_Source.xlsx
+++ b/Sterlco _4300_Series_Condensate_Duplex_Source.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a634b9d077ee98e5/Desktop/Shopify/Sterlco All Products/Sterlco/4300_SC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a634b9d077ee98e5/Desktop/Shopify_CLI_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{55C10578-B7F3-442C-8F9C-EE04BFA173B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77F8D0F5-4274-4B99-9991-37881AA89E4F}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="8_{55C10578-B7F3-442C-8F9C-EE04BFA173B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E48AB444-A4FC-4670-A1D8-D804C6513A79}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{82AB6ACC-2189-47E7-8F65-11FDCF6C4331}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{82AB6ACC-2189-47E7-8F65-11FDCF6C4331}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -559,7 +559,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>